<commit_message>
Desafio1 de power bi dashborad financial
</commit_message>
<xml_diff>
--- a/excel e copilot/Vendas_Xbox/Base_Vendas_Xbox.xlsx
+++ b/excel e copilot/Vendas_Xbox/Base_Vendas_Xbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e131bea2c3470e5e/Desktop/Fábio/botcamp_PowerBI/Bootcamp_PowerBI/excel e copilot/Vendas_Xbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="429" documentId="13_ncr:1_{3C2F8ED6-40B2-4E08-832A-7140AC03FA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9430B62D-169C-4138-98FF-9D6545622BB8}"/>
+  <xr:revisionPtr revIDLastSave="434" documentId="13_ncr:1_{3C2F8ED6-40B2-4E08-832A-7140AC03FA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30D364DF-B38E-4C6B-882D-B4DFE80253C3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="746" firstSheet="3" activeTab="3" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
   </bookViews>
@@ -3428,8 +3428,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1785938" y="154783"/>
-          <a:ext cx="523875" cy="596368"/>
+          <a:off x="1791040" y="154783"/>
+          <a:ext cx="530679" cy="599769"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -22105,7 +22105,7 @@
   <dimension ref="A2:P200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+      <selection activeCell="C4" sqref="C4:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>